<commit_message>
- Add a missing ask in AppFragment to let readOne in Dispatch typecheck - Update the report: Encode and StatefulLHAE are typechecking
</commit_message>
<xml_diff>
--- a/lib/REPORT_2013_09_23.xlsx
+++ b/lib/REPORT_2013_09_23.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>TLSError</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>1 ask about Open</t>
-  </si>
-  <si>
-    <t>arithmetic -- OK in why3 (alt-ergo used for the failing arithmetic query)</t>
   </si>
   <si>
     <t>1 ask -- unbound symbol 'v_Tuples__Tup0' in why3</t>
@@ -534,7 +531,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,7 +623,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,7 +661,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,10 +733,7 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,7 +777,7 @@
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,7 +785,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +812,7 @@
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -864,7 +858,7 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -875,7 +869,7 @@
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,7 +880,7 @@
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -905,7 +899,7 @@
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,7 +910,7 @@
         <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>